<commit_message>
Added secondary resources from NSB
</commit_message>
<xml_diff>
--- a/data/scenario_data/Energy_storage_demand.xlsx
+++ b/data/scenario_data/Energy_storage_demand.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="7">
   <si>
     <t>index</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>CP4All</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D304"/>
+  <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1355,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>0.05161155183774097</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1369,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>0.08503612057176439</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1383,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>0.1400463483560487</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1397,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>0.2304786089687104</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1411,7 +1414,7 @@
         <v>3</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>0.3788620633930405</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2769,7 +2772,7 @@
         <v>4</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>0.06834730452848502</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2783,7 +2786,7 @@
         <v>4</v>
       </c>
       <c r="D171">
-        <v>0</v>
+        <v>0.1126269054631187</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2797,7 +2800,7 @@
         <v>4</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>0.1855308978543403</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2811,7 +2814,7 @@
         <v>4</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>0.3054562194207077</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2825,7 +2828,7 @@
         <v>4</v>
       </c>
       <c r="D174">
-        <v>0</v>
+        <v>0.5024408527807227</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4183,7 +4186,7 @@
         <v>5</v>
       </c>
       <c r="D271">
-        <v>0</v>
+        <v>0.08952346006039959</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4197,7 +4200,7 @@
         <v>5</v>
       </c>
       <c r="D272">
-        <v>0</v>
+        <v>0.1475278345532837</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4211,7 +4214,7 @@
         <v>5</v>
       </c>
       <c r="D273">
-        <v>0</v>
+        <v>0.2430384466859748</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4225,7 +4228,7 @@
         <v>5</v>
       </c>
       <c r="D274">
-        <v>0</v>
+        <v>0.4001768768895833</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4239,7 +4242,7 @@
         <v>5</v>
       </c>
       <c r="D275">
-        <v>0</v>
+        <v>0.6583558679340189</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4646,6 +4649,1420 @@
       </c>
       <c r="D304">
         <v>119.9890300951377</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="A305" s="1">
+        <v>303</v>
+      </c>
+      <c r="B305">
+        <v>1950</v>
+      </c>
+      <c r="C305" t="s">
+        <v>6</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306" s="1">
+        <v>304</v>
+      </c>
+      <c r="B306">
+        <v>1951</v>
+      </c>
+      <c r="C306" t="s">
+        <v>6</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="A307" s="1">
+        <v>305</v>
+      </c>
+      <c r="B307">
+        <v>1952</v>
+      </c>
+      <c r="C307" t="s">
+        <v>6</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4">
+      <c r="A308" s="1">
+        <v>306</v>
+      </c>
+      <c r="B308">
+        <v>1953</v>
+      </c>
+      <c r="C308" t="s">
+        <v>6</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309" s="1">
+        <v>307</v>
+      </c>
+      <c r="B309">
+        <v>1954</v>
+      </c>
+      <c r="C309" t="s">
+        <v>6</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="A310" s="1">
+        <v>308</v>
+      </c>
+      <c r="B310">
+        <v>1955</v>
+      </c>
+      <c r="C310" t="s">
+        <v>6</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
+      <c r="A311" s="1">
+        <v>309</v>
+      </c>
+      <c r="B311">
+        <v>1956</v>
+      </c>
+      <c r="C311" t="s">
+        <v>6</v>
+      </c>
+      <c r="D311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="A312" s="1">
+        <v>310</v>
+      </c>
+      <c r="B312">
+        <v>1957</v>
+      </c>
+      <c r="C312" t="s">
+        <v>6</v>
+      </c>
+      <c r="D312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
+      <c r="A313" s="1">
+        <v>311</v>
+      </c>
+      <c r="B313">
+        <v>1958</v>
+      </c>
+      <c r="C313" t="s">
+        <v>6</v>
+      </c>
+      <c r="D313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
+      <c r="A314" s="1">
+        <v>312</v>
+      </c>
+      <c r="B314">
+        <v>1959</v>
+      </c>
+      <c r="C314" t="s">
+        <v>6</v>
+      </c>
+      <c r="D314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
+      <c r="A315" s="1">
+        <v>313</v>
+      </c>
+      <c r="B315">
+        <v>1960</v>
+      </c>
+      <c r="C315" t="s">
+        <v>6</v>
+      </c>
+      <c r="D315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
+      <c r="A316" s="1">
+        <v>314</v>
+      </c>
+      <c r="B316">
+        <v>1961</v>
+      </c>
+      <c r="C316" t="s">
+        <v>6</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4">
+      <c r="A317" s="1">
+        <v>315</v>
+      </c>
+      <c r="B317">
+        <v>1962</v>
+      </c>
+      <c r="C317" t="s">
+        <v>6</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4">
+      <c r="A318" s="1">
+        <v>316</v>
+      </c>
+      <c r="B318">
+        <v>1963</v>
+      </c>
+      <c r="C318" t="s">
+        <v>6</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
+      <c r="A319" s="1">
+        <v>317</v>
+      </c>
+      <c r="B319">
+        <v>1964</v>
+      </c>
+      <c r="C319" t="s">
+        <v>6</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4">
+      <c r="A320" s="1">
+        <v>318</v>
+      </c>
+      <c r="B320">
+        <v>1965</v>
+      </c>
+      <c r="C320" t="s">
+        <v>6</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4">
+      <c r="A321" s="1">
+        <v>319</v>
+      </c>
+      <c r="B321">
+        <v>1966</v>
+      </c>
+      <c r="C321" t="s">
+        <v>6</v>
+      </c>
+      <c r="D321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4">
+      <c r="A322" s="1">
+        <v>320</v>
+      </c>
+      <c r="B322">
+        <v>1967</v>
+      </c>
+      <c r="C322" t="s">
+        <v>6</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4">
+      <c r="A323" s="1">
+        <v>321</v>
+      </c>
+      <c r="B323">
+        <v>1968</v>
+      </c>
+      <c r="C323" t="s">
+        <v>6</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4">
+      <c r="A324" s="1">
+        <v>322</v>
+      </c>
+      <c r="B324">
+        <v>1969</v>
+      </c>
+      <c r="C324" t="s">
+        <v>6</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4">
+      <c r="A325" s="1">
+        <v>323</v>
+      </c>
+      <c r="B325">
+        <v>1970</v>
+      </c>
+      <c r="C325" t="s">
+        <v>6</v>
+      </c>
+      <c r="D325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4">
+      <c r="A326" s="1">
+        <v>324</v>
+      </c>
+      <c r="B326">
+        <v>1971</v>
+      </c>
+      <c r="C326" t="s">
+        <v>6</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4">
+      <c r="A327" s="1">
+        <v>325</v>
+      </c>
+      <c r="B327">
+        <v>1972</v>
+      </c>
+      <c r="C327" t="s">
+        <v>6</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4">
+      <c r="A328" s="1">
+        <v>326</v>
+      </c>
+      <c r="B328">
+        <v>1973</v>
+      </c>
+      <c r="C328" t="s">
+        <v>6</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4">
+      <c r="A329" s="1">
+        <v>327</v>
+      </c>
+      <c r="B329">
+        <v>1974</v>
+      </c>
+      <c r="C329" t="s">
+        <v>6</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4">
+      <c r="A330" s="1">
+        <v>328</v>
+      </c>
+      <c r="B330">
+        <v>1975</v>
+      </c>
+      <c r="C330" t="s">
+        <v>6</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4">
+      <c r="A331" s="1">
+        <v>329</v>
+      </c>
+      <c r="B331">
+        <v>1976</v>
+      </c>
+      <c r="C331" t="s">
+        <v>6</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4">
+      <c r="A332" s="1">
+        <v>330</v>
+      </c>
+      <c r="B332">
+        <v>1977</v>
+      </c>
+      <c r="C332" t="s">
+        <v>6</v>
+      </c>
+      <c r="D332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4">
+      <c r="A333" s="1">
+        <v>331</v>
+      </c>
+      <c r="B333">
+        <v>1978</v>
+      </c>
+      <c r="C333" t="s">
+        <v>6</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4">
+      <c r="A334" s="1">
+        <v>332</v>
+      </c>
+      <c r="B334">
+        <v>1979</v>
+      </c>
+      <c r="C334" t="s">
+        <v>6</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4">
+      <c r="A335" s="1">
+        <v>333</v>
+      </c>
+      <c r="B335">
+        <v>1980</v>
+      </c>
+      <c r="C335" t="s">
+        <v>6</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4">
+      <c r="A336" s="1">
+        <v>334</v>
+      </c>
+      <c r="B336">
+        <v>1981</v>
+      </c>
+      <c r="C336" t="s">
+        <v>6</v>
+      </c>
+      <c r="D336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4">
+      <c r="A337" s="1">
+        <v>335</v>
+      </c>
+      <c r="B337">
+        <v>1982</v>
+      </c>
+      <c r="C337" t="s">
+        <v>6</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4">
+      <c r="A338" s="1">
+        <v>336</v>
+      </c>
+      <c r="B338">
+        <v>1983</v>
+      </c>
+      <c r="C338" t="s">
+        <v>6</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4">
+      <c r="A339" s="1">
+        <v>337</v>
+      </c>
+      <c r="B339">
+        <v>1984</v>
+      </c>
+      <c r="C339" t="s">
+        <v>6</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4">
+      <c r="A340" s="1">
+        <v>338</v>
+      </c>
+      <c r="B340">
+        <v>1985</v>
+      </c>
+      <c r="C340" t="s">
+        <v>6</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4">
+      <c r="A341" s="1">
+        <v>339</v>
+      </c>
+      <c r="B341">
+        <v>1986</v>
+      </c>
+      <c r="C341" t="s">
+        <v>6</v>
+      </c>
+      <c r="D341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4">
+      <c r="A342" s="1">
+        <v>340</v>
+      </c>
+      <c r="B342">
+        <v>1987</v>
+      </c>
+      <c r="C342" t="s">
+        <v>6</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4">
+      <c r="A343" s="1">
+        <v>341</v>
+      </c>
+      <c r="B343">
+        <v>1988</v>
+      </c>
+      <c r="C343" t="s">
+        <v>6</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4">
+      <c r="A344" s="1">
+        <v>342</v>
+      </c>
+      <c r="B344">
+        <v>1989</v>
+      </c>
+      <c r="C344" t="s">
+        <v>6</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4">
+      <c r="A345" s="1">
+        <v>343</v>
+      </c>
+      <c r="B345">
+        <v>1990</v>
+      </c>
+      <c r="C345" t="s">
+        <v>6</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4">
+      <c r="A346" s="1">
+        <v>344</v>
+      </c>
+      <c r="B346">
+        <v>1991</v>
+      </c>
+      <c r="C346" t="s">
+        <v>6</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4">
+      <c r="A347" s="1">
+        <v>345</v>
+      </c>
+      <c r="B347">
+        <v>1992</v>
+      </c>
+      <c r="C347" t="s">
+        <v>6</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4">
+      <c r="A348" s="1">
+        <v>346</v>
+      </c>
+      <c r="B348">
+        <v>1993</v>
+      </c>
+      <c r="C348" t="s">
+        <v>6</v>
+      </c>
+      <c r="D348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4">
+      <c r="A349" s="1">
+        <v>347</v>
+      </c>
+      <c r="B349">
+        <v>1994</v>
+      </c>
+      <c r="C349" t="s">
+        <v>6</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4">
+      <c r="A350" s="1">
+        <v>348</v>
+      </c>
+      <c r="B350">
+        <v>1995</v>
+      </c>
+      <c r="C350" t="s">
+        <v>6</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4">
+      <c r="A351" s="1">
+        <v>349</v>
+      </c>
+      <c r="B351">
+        <v>1996</v>
+      </c>
+      <c r="C351" t="s">
+        <v>6</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4">
+      <c r="A352" s="1">
+        <v>350</v>
+      </c>
+      <c r="B352">
+        <v>1997</v>
+      </c>
+      <c r="C352" t="s">
+        <v>6</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4">
+      <c r="A353" s="1">
+        <v>351</v>
+      </c>
+      <c r="B353">
+        <v>1998</v>
+      </c>
+      <c r="C353" t="s">
+        <v>6</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4">
+      <c r="A354" s="1">
+        <v>352</v>
+      </c>
+      <c r="B354">
+        <v>1999</v>
+      </c>
+      <c r="C354" t="s">
+        <v>6</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4">
+      <c r="A355" s="1">
+        <v>353</v>
+      </c>
+      <c r="B355">
+        <v>2000</v>
+      </c>
+      <c r="C355" t="s">
+        <v>6</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4">
+      <c r="A356" s="1">
+        <v>354</v>
+      </c>
+      <c r="B356">
+        <v>2001</v>
+      </c>
+      <c r="C356" t="s">
+        <v>6</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4">
+      <c r="A357" s="1">
+        <v>355</v>
+      </c>
+      <c r="B357">
+        <v>2002</v>
+      </c>
+      <c r="C357" t="s">
+        <v>6</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4">
+      <c r="A358" s="1">
+        <v>356</v>
+      </c>
+      <c r="B358">
+        <v>2003</v>
+      </c>
+      <c r="C358" t="s">
+        <v>6</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4">
+      <c r="A359" s="1">
+        <v>357</v>
+      </c>
+      <c r="B359">
+        <v>2004</v>
+      </c>
+      <c r="C359" t="s">
+        <v>6</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4">
+      <c r="A360" s="1">
+        <v>358</v>
+      </c>
+      <c r="B360">
+        <v>2005</v>
+      </c>
+      <c r="C360" t="s">
+        <v>6</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4">
+      <c r="A361" s="1">
+        <v>359</v>
+      </c>
+      <c r="B361">
+        <v>2006</v>
+      </c>
+      <c r="C361" t="s">
+        <v>6</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4">
+      <c r="A362" s="1">
+        <v>360</v>
+      </c>
+      <c r="B362">
+        <v>2007</v>
+      </c>
+      <c r="C362" t="s">
+        <v>6</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4">
+      <c r="A363" s="1">
+        <v>361</v>
+      </c>
+      <c r="B363">
+        <v>2008</v>
+      </c>
+      <c r="C363" t="s">
+        <v>6</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4">
+      <c r="A364" s="1">
+        <v>362</v>
+      </c>
+      <c r="B364">
+        <v>2009</v>
+      </c>
+      <c r="C364" t="s">
+        <v>6</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4">
+      <c r="A365" s="1">
+        <v>363</v>
+      </c>
+      <c r="B365">
+        <v>2010</v>
+      </c>
+      <c r="C365" t="s">
+        <v>6</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4">
+      <c r="A366" s="1">
+        <v>364</v>
+      </c>
+      <c r="B366">
+        <v>2011</v>
+      </c>
+      <c r="C366" t="s">
+        <v>6</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4">
+      <c r="A367" s="1">
+        <v>365</v>
+      </c>
+      <c r="B367">
+        <v>2012</v>
+      </c>
+      <c r="C367" t="s">
+        <v>6</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4">
+      <c r="A368" s="1">
+        <v>366</v>
+      </c>
+      <c r="B368">
+        <v>2013</v>
+      </c>
+      <c r="C368" t="s">
+        <v>6</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4">
+      <c r="A369" s="1">
+        <v>367</v>
+      </c>
+      <c r="B369">
+        <v>2014</v>
+      </c>
+      <c r="C369" t="s">
+        <v>6</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4">
+      <c r="A370" s="1">
+        <v>368</v>
+      </c>
+      <c r="B370">
+        <v>2015</v>
+      </c>
+      <c r="C370" t="s">
+        <v>6</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4">
+      <c r="A371" s="1">
+        <v>369</v>
+      </c>
+      <c r="B371">
+        <v>2016</v>
+      </c>
+      <c r="C371" t="s">
+        <v>6</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4">
+      <c r="A372" s="1">
+        <v>370</v>
+      </c>
+      <c r="B372">
+        <v>2017</v>
+      </c>
+      <c r="C372" t="s">
+        <v>6</v>
+      </c>
+      <c r="D372">
+        <v>0.2002564859148577</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4">
+      <c r="A373" s="1">
+        <v>371</v>
+      </c>
+      <c r="B373">
+        <v>2018</v>
+      </c>
+      <c r="C373" t="s">
+        <v>6</v>
+      </c>
+      <c r="D373">
+        <v>0.2985841944313958</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4">
+      <c r="A374" s="1">
+        <v>372</v>
+      </c>
+      <c r="B374">
+        <v>2019</v>
+      </c>
+      <c r="C374" t="s">
+        <v>6</v>
+      </c>
+      <c r="D374">
+        <v>0.4450721681942594</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4">
+      <c r="A375" s="1">
+        <v>373</v>
+      </c>
+      <c r="B375">
+        <v>2020</v>
+      </c>
+      <c r="C375" t="s">
+        <v>6</v>
+      </c>
+      <c r="D375">
+        <v>0.6631631818984774</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4">
+      <c r="A376" s="1">
+        <v>374</v>
+      </c>
+      <c r="B376">
+        <v>2021</v>
+      </c>
+      <c r="C376" t="s">
+        <v>6</v>
+      </c>
+      <c r="D376">
+        <v>0.9875338019010728</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4">
+      <c r="A377" s="1">
+        <v>375</v>
+      </c>
+      <c r="B377">
+        <v>2022</v>
+      </c>
+      <c r="C377" t="s">
+        <v>6</v>
+      </c>
+      <c r="D377">
+        <v>1.46926280756878</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4">
+      <c r="A378" s="1">
+        <v>376</v>
+      </c>
+      <c r="B378">
+        <v>2023</v>
+      </c>
+      <c r="C378" t="s">
+        <v>6</v>
+      </c>
+      <c r="D378">
+        <v>2.183118297169362</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4">
+      <c r="A379" s="1">
+        <v>377</v>
+      </c>
+      <c r="B379">
+        <v>2024</v>
+      </c>
+      <c r="C379" t="s">
+        <v>6</v>
+      </c>
+      <c r="D379">
+        <v>3.23751779317648</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4">
+      <c r="A380" s="1">
+        <v>378</v>
+      </c>
+      <c r="B380">
+        <v>2025</v>
+      </c>
+      <c r="C380" t="s">
+        <v>6</v>
+      </c>
+      <c r="D380">
+        <v>4.787458843835854</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4">
+      <c r="A381" s="1">
+        <v>379</v>
+      </c>
+      <c r="B381">
+        <v>2026</v>
+      </c>
+      <c r="C381" t="s">
+        <v>6</v>
+      </c>
+      <c r="D381">
+        <v>7.049830103417584</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4">
+      <c r="A382" s="1">
+        <v>380</v>
+      </c>
+      <c r="B382">
+        <v>2027</v>
+      </c>
+      <c r="C382" t="s">
+        <v>6</v>
+      </c>
+      <c r="D382">
+        <v>10.31835166179637</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4">
+      <c r="A383" s="1">
+        <v>381</v>
+      </c>
+      <c r="B383">
+        <v>2028</v>
+      </c>
+      <c r="C383" t="s">
+        <v>6</v>
+      </c>
+      <c r="D383">
+        <v>14.97108536890602</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4">
+      <c r="A384" s="1">
+        <v>382</v>
+      </c>
+      <c r="B384">
+        <v>2029</v>
+      </c>
+      <c r="C384" t="s">
+        <v>6</v>
+      </c>
+      <c r="D384">
+        <v>21.45652596398116</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4">
+      <c r="A385" s="1">
+        <v>383</v>
+      </c>
+      <c r="B385">
+        <v>2030</v>
+      </c>
+      <c r="C385" t="s">
+        <v>6</v>
+      </c>
+      <c r="D385">
+        <v>30.23669067589359</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4">
+      <c r="A386" s="1">
+        <v>384</v>
+      </c>
+      <c r="B386">
+        <v>2031</v>
+      </c>
+      <c r="C386" t="s">
+        <v>6</v>
+      </c>
+      <c r="D386">
+        <v>41.66553897017682</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4">
+      <c r="A387" s="1">
+        <v>385</v>
+      </c>
+      <c r="B387">
+        <v>2032</v>
+      </c>
+      <c r="C387" t="s">
+        <v>6</v>
+      </c>
+      <c r="D387">
+        <v>55.80459339702976</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4">
+      <c r="A388" s="1">
+        <v>386</v>
+      </c>
+      <c r="B388">
+        <v>2033</v>
+      </c>
+      <c r="C388" t="s">
+        <v>6</v>
+      </c>
+      <c r="D388">
+        <v>72.23622117975864</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4">
+      <c r="A389" s="1">
+        <v>387</v>
+      </c>
+      <c r="B389">
+        <v>2034</v>
+      </c>
+      <c r="C389" t="s">
+        <v>6</v>
+      </c>
+      <c r="D389">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4">
+      <c r="A390" s="1">
+        <v>388</v>
+      </c>
+      <c r="B390">
+        <v>2035</v>
+      </c>
+      <c r="C390" t="s">
+        <v>6</v>
+      </c>
+      <c r="D390">
+        <v>107.7637788202414</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4">
+      <c r="A391" s="1">
+        <v>389</v>
+      </c>
+      <c r="B391">
+        <v>2036</v>
+      </c>
+      <c r="C391" t="s">
+        <v>6</v>
+      </c>
+      <c r="D391">
+        <v>124.1954066029702</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4">
+      <c r="A392" s="1">
+        <v>390</v>
+      </c>
+      <c r="B392">
+        <v>2037</v>
+      </c>
+      <c r="C392" t="s">
+        <v>6</v>
+      </c>
+      <c r="D392">
+        <v>138.3344610298232</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4">
+      <c r="A393" s="1">
+        <v>391</v>
+      </c>
+      <c r="B393">
+        <v>2038</v>
+      </c>
+      <c r="C393" t="s">
+        <v>6</v>
+      </c>
+      <c r="D393">
+        <v>149.7633093241064</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4">
+      <c r="A394" s="1">
+        <v>392</v>
+      </c>
+      <c r="B394">
+        <v>2039</v>
+      </c>
+      <c r="C394" t="s">
+        <v>6</v>
+      </c>
+      <c r="D394">
+        <v>158.5434740360188</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4">
+      <c r="A395" s="1">
+        <v>393</v>
+      </c>
+      <c r="B395">
+        <v>2040</v>
+      </c>
+      <c r="C395" t="s">
+        <v>6</v>
+      </c>
+      <c r="D395">
+        <v>165.028914631094</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4">
+      <c r="A396" s="1">
+        <v>394</v>
+      </c>
+      <c r="B396">
+        <v>2041</v>
+      </c>
+      <c r="C396" t="s">
+        <v>6</v>
+      </c>
+      <c r="D396">
+        <v>169.6816483382036</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4">
+      <c r="A397" s="1">
+        <v>395</v>
+      </c>
+      <c r="B397">
+        <v>2042</v>
+      </c>
+      <c r="C397" t="s">
+        <v>6</v>
+      </c>
+      <c r="D397">
+        <v>172.9501698965824</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4">
+      <c r="A398" s="1">
+        <v>396</v>
+      </c>
+      <c r="B398">
+        <v>2043</v>
+      </c>
+      <c r="C398" t="s">
+        <v>6</v>
+      </c>
+      <c r="D398">
+        <v>175.2125411561641</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4">
+      <c r="A399" s="1">
+        <v>397</v>
+      </c>
+      <c r="B399">
+        <v>2044</v>
+      </c>
+      <c r="C399" t="s">
+        <v>6</v>
+      </c>
+      <c r="D399">
+        <v>176.7624822068235</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4">
+      <c r="A400" s="1">
+        <v>398</v>
+      </c>
+      <c r="B400">
+        <v>2045</v>
+      </c>
+      <c r="C400" t="s">
+        <v>6</v>
+      </c>
+      <c r="D400">
+        <v>177.8168817028306</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4">
+      <c r="A401" s="1">
+        <v>399</v>
+      </c>
+      <c r="B401">
+        <v>2046</v>
+      </c>
+      <c r="C401" t="s">
+        <v>6</v>
+      </c>
+      <c r="D401">
+        <v>178.5307371924312</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4">
+      <c r="A402" s="1">
+        <v>400</v>
+      </c>
+      <c r="B402">
+        <v>2047</v>
+      </c>
+      <c r="C402" t="s">
+        <v>6</v>
+      </c>
+      <c r="D402">
+        <v>179.0124661980989</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4">
+      <c r="A403" s="1">
+        <v>401</v>
+      </c>
+      <c r="B403">
+        <v>2048</v>
+      </c>
+      <c r="C403" t="s">
+        <v>6</v>
+      </c>
+      <c r="D403">
+        <v>179.3368368181015</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4">
+      <c r="A404" s="1">
+        <v>402</v>
+      </c>
+      <c r="B404">
+        <v>2049</v>
+      </c>
+      <c r="C404" t="s">
+        <v>6</v>
+      </c>
+      <c r="D404">
+        <v>179.5549278318058</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4">
+      <c r="A405" s="1">
+        <v>403</v>
+      </c>
+      <c r="B405">
+        <v>2050</v>
+      </c>
+      <c r="C405" t="s">
+        <v>6</v>
+      </c>
+      <c r="D405">
+        <v>179.7014158055686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>